<commit_message>
Till Monday - 14-06-2021
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\RTA_Github\RTA_DNM\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -306,16 +311,16 @@
     <t>N</t>
   </si>
   <si>
-    <t>D:\RTA\RTA_FrameworkTemplate\Data\Input\TestCases.xlsx</t>
-  </si>
-  <si>
     <t xml:space="preserve">Test DNM </t>
+  </si>
+  <si>
+    <t>F:\RTA_Github\RTA_DNM\Data\Input\TestCases.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -733,24 +738,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1013"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="2" max="2" width="56.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="88.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
@@ -846,7 +851,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C7" t="s">
         <v>47</v>
@@ -1085,7 +1090,7 @@
         <v>77</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C50" t="s">
         <v>78</v>
@@ -2160,7 +2165,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z987"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3272,7 +3277,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
After Client Demo on 21-06-21 at 7 pm
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -748,14 +748,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1013"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="56.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43" customWidth="1"/>
     <col min="3" max="3" width="88.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>

</xml_diff>